<commit_message>
added continuous radial distribution function
</commit_message>
<xml_diff>
--- a/Results/Benchmarking.xlsx
+++ b/Results/Benchmarking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="0" windowWidth="7395" windowHeight="1170" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="0" windowWidth="7395" windowHeight="1170"/>
   </bookViews>
   <sheets>
     <sheet name="Event-Driven" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
   <si>
     <t>Simulation Benchmarking</t>
   </si>
@@ -124,6 +124,39 @@
   </si>
   <si>
     <t>ratio U</t>
+  </si>
+  <si>
+    <t>Stepped Potentials</t>
+  </si>
+  <si>
+    <t>Results from Chapela</t>
+  </si>
+  <si>
+    <t>Ud</t>
+  </si>
+  <si>
+    <t>Pd</t>
+  </si>
+  <si>
+    <t>Case 6 results</t>
+  </si>
+  <si>
+    <t>256 Particles</t>
+  </si>
+  <si>
+    <t>1.5 million Collisions</t>
+  </si>
+  <si>
+    <t>1 million samples</t>
+  </si>
+  <si>
+    <t>Ud(sd)</t>
+  </si>
+  <si>
+    <t>Pd(sd)</t>
+  </si>
+  <si>
+    <t>%difference</t>
   </si>
 </sst>
 </file>
@@ -170,10 +203,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -207,7 +241,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-0.44046879854303927"/>
-                  <c:y val="-3.5504011022483364E-2"/>
+                  <c:y val="-3.5504011022483371E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -292,22 +326,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="75612544"/>
-        <c:axId val="126509824"/>
+        <c:axId val="97252096"/>
+        <c:axId val="97253632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75612544"/>
+        <c:axId val="97252096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126509824"/>
+        <c:crossAx val="97253632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="126509824"/>
+        <c:axId val="97253632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -315,7 +349,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75612544"/>
+        <c:crossAx val="97252096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -333,7 +367,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -659,13 +693,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
@@ -1041,6 +1078,644 @@
       <c r="O15" s="1">
         <f t="shared" si="4"/>
         <v>9.1324200913242507E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="D20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" t="s">
+        <v>42</v>
+      </c>
+      <c r="K20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G22" t="s">
+        <v>25</v>
+      </c>
+      <c r="O22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" t="s">
+        <v>3</v>
+      </c>
+      <c r="H24" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" t="s">
+        <v>38</v>
+      </c>
+      <c r="K24" t="s">
+        <v>44</v>
+      </c>
+      <c r="L24" t="s">
+        <v>39</v>
+      </c>
+      <c r="M24" t="s">
+        <v>45</v>
+      </c>
+      <c r="O24" t="s">
+        <v>17</v>
+      </c>
+      <c r="P24" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25">
+        <v>0.85</v>
+      </c>
+      <c r="B25">
+        <v>0.72</v>
+      </c>
+      <c r="C25" s="3">
+        <v>-5.8</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.54</v>
+      </c>
+      <c r="G25">
+        <v>0.85</v>
+      </c>
+      <c r="H25">
+        <v>0.71931699999999998</v>
+      </c>
+      <c r="I25">
+        <v>3.8024599999999999E-2</v>
+      </c>
+      <c r="J25">
+        <v>-6.0938699999999999</v>
+      </c>
+      <c r="K25">
+        <v>6.23492E-2</v>
+      </c>
+      <c r="L25">
+        <v>-0.78096600000000005</v>
+      </c>
+      <c r="M25">
+        <v>3.23209E-2</v>
+      </c>
+      <c r="O25" s="1">
+        <f>(B25-H25)*2/(B25+H25)</f>
+        <v>9.4906125613744465E-4</v>
+      </c>
+      <c r="P25" s="1">
+        <f>(C25-J25)*2/(C25+J25)</f>
+        <v>-4.9415371111337196E-2</v>
+      </c>
+      <c r="Q25" s="1">
+        <f>(D25-L25)*2/(D25+L25)</f>
+        <v>-10.963920221110032</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26">
+        <v>0.85</v>
+      </c>
+      <c r="B26">
+        <v>1.34</v>
+      </c>
+      <c r="C26" s="3">
+        <v>-5.14</v>
+      </c>
+      <c r="D26" s="3">
+        <v>4.08</v>
+      </c>
+      <c r="G26">
+        <v>0.85</v>
+      </c>
+      <c r="H26">
+        <v>1.34127</v>
+      </c>
+      <c r="I26">
+        <v>6.6176899999999997E-2</v>
+      </c>
+      <c r="J26">
+        <v>-5.1227499999999999</v>
+      </c>
+      <c r="K26">
+        <v>7.76009E-2</v>
+      </c>
+      <c r="L26">
+        <v>4.1493200000000003</v>
+      </c>
+      <c r="M26">
+        <v>5.8250400000000001E-2</v>
+      </c>
+      <c r="O26" s="1">
+        <f t="shared" ref="O26:O36" si="5">(B26-H26)*2/(B26+H26)</f>
+        <v>-9.4731228112042605E-4</v>
+      </c>
+      <c r="P26" s="1">
+        <f t="shared" ref="P26:P36" si="6">(C26-J26)*2/(C26+J26)</f>
+        <v>3.3616720664538771E-3</v>
+      </c>
+      <c r="Q26" s="1">
+        <f t="shared" ref="Q26:Q36" si="7">(D26-L26)*2/(D26+L26)</f>
+        <v>-1.6847078494942536E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27">
+        <v>0.85</v>
+      </c>
+      <c r="B27">
+        <v>2.35</v>
+      </c>
+      <c r="C27" s="3">
+        <v>-4.2</v>
+      </c>
+      <c r="D27" s="3">
+        <v>8.86</v>
+      </c>
+      <c r="G27">
+        <v>0.85</v>
+      </c>
+      <c r="H27">
+        <v>2.3424200000000002</v>
+      </c>
+      <c r="I27">
+        <v>0.116746</v>
+      </c>
+      <c r="J27">
+        <v>-4.2613000000000003</v>
+      </c>
+      <c r="K27">
+        <v>0.118004</v>
+      </c>
+      <c r="L27">
+        <v>8.7375699999999998</v>
+      </c>
+      <c r="M27">
+        <v>9.92339E-2</v>
+      </c>
+      <c r="O27" s="1">
+        <f t="shared" si="5"/>
+        <v>3.2307423461667623E-3</v>
+      </c>
+      <c r="P27" s="1">
+        <f t="shared" si="6"/>
+        <v>-1.4489499249524333E-2</v>
+      </c>
+      <c r="Q27" s="1">
+        <f t="shared" si="7"/>
+        <v>1.3914421138827647E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28">
+        <v>0.85</v>
+      </c>
+      <c r="B28">
+        <v>3.37</v>
+      </c>
+      <c r="C28" s="3">
+        <v>-3.49</v>
+      </c>
+      <c r="D28" s="3">
+        <v>13</v>
+      </c>
+      <c r="G28">
+        <v>0.85</v>
+      </c>
+      <c r="H28">
+        <v>3.3837899999999999</v>
+      </c>
+      <c r="I28">
+        <v>0.15849199999999999</v>
+      </c>
+      <c r="J28">
+        <v>-3.4720200000000001</v>
+      </c>
+      <c r="K28">
+        <v>0.16657</v>
+      </c>
+      <c r="L28">
+        <v>12.9101</v>
+      </c>
+      <c r="M28">
+        <v>0.134718</v>
+      </c>
+      <c r="O28" s="1">
+        <f t="shared" si="5"/>
+        <v>-4.0836330415958289E-3</v>
+      </c>
+      <c r="P28" s="1">
+        <f t="shared" si="6"/>
+        <v>5.1651675806734555E-3</v>
+      </c>
+      <c r="Q28" s="1">
+        <f t="shared" si="7"/>
+        <v>6.9393788522622525E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29">
+        <v>0.85</v>
+      </c>
+      <c r="B29">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C29" s="3">
+        <v>-2.68</v>
+      </c>
+      <c r="D29" s="3">
+        <v>13.43</v>
+      </c>
+      <c r="G29">
+        <v>0.85</v>
+      </c>
+      <c r="H29">
+        <v>4.6173599999999997</v>
+      </c>
+      <c r="I29">
+        <v>0.20890500000000001</v>
+      </c>
+      <c r="J29">
+        <v>-2.6463100000000002</v>
+      </c>
+      <c r="K29">
+        <v>0.21601300000000001</v>
+      </c>
+      <c r="L29">
+        <v>17.3596</v>
+      </c>
+      <c r="M29">
+        <v>0.177569</v>
+      </c>
+      <c r="O29" s="1">
+        <f t="shared" si="5"/>
+        <v>-3.7668052457536742E-3</v>
+      </c>
+      <c r="P29" s="1">
+        <f t="shared" si="6"/>
+        <v>1.2650409007361568E-2</v>
+      </c>
+      <c r="Q29" s="1">
+        <f t="shared" si="7"/>
+        <v>-0.25525502117598153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30">
+        <v>0.75</v>
+      </c>
+      <c r="B30">
+        <v>0.81</v>
+      </c>
+      <c r="C30" s="3">
+        <v>-5.08</v>
+      </c>
+      <c r="D30" s="3">
+        <v>-0.24</v>
+      </c>
+      <c r="G30">
+        <v>0.75</v>
+      </c>
+      <c r="H30">
+        <v>0.81188400000000005</v>
+      </c>
+      <c r="I30">
+        <v>3.9287099999999998E-2</v>
+      </c>
+      <c r="J30">
+        <v>-5.0942100000000003</v>
+      </c>
+      <c r="K30">
+        <v>4.8450100000000003E-2</v>
+      </c>
+      <c r="L30">
+        <v>-0.19492799999999999</v>
+      </c>
+      <c r="M30">
+        <v>2.94653E-2</v>
+      </c>
+      <c r="O30" s="1">
+        <f t="shared" si="5"/>
+        <v>-2.3232241023402374E-3</v>
+      </c>
+      <c r="P30" s="1">
+        <f t="shared" si="6"/>
+        <v>-2.7933372713950817E-3</v>
+      </c>
+      <c r="Q30" s="1">
+        <f t="shared" si="7"/>
+        <v>0.20726189162344114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31">
+        <v>0.75</v>
+      </c>
+      <c r="B31">
+        <v>1.31</v>
+      </c>
+      <c r="C31" s="3">
+        <v>-4.63</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1.84</v>
+      </c>
+      <c r="G31">
+        <v>0.75</v>
+      </c>
+      <c r="H31">
+        <v>1.31273</v>
+      </c>
+      <c r="I31">
+        <v>7.0916199999999999E-2</v>
+      </c>
+      <c r="J31">
+        <v>-4.6621499999999996</v>
+      </c>
+      <c r="K31">
+        <v>7.4607800000000002E-2</v>
+      </c>
+      <c r="L31">
+        <v>1.8208500000000001</v>
+      </c>
+      <c r="M31">
+        <v>5.3187100000000001E-2</v>
+      </c>
+      <c r="O31" s="1">
+        <f t="shared" si="5"/>
+        <v>-2.0818002615594433E-3</v>
+      </c>
+      <c r="P31" s="1">
+        <f t="shared" si="6"/>
+        <v>-6.9198194174652115E-3</v>
+      </c>
+      <c r="Q31" s="1">
+        <f t="shared" si="7"/>
+        <v>1.0462051162981276E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="A32">
+        <v>0.75</v>
+      </c>
+      <c r="B32">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="C32" s="3">
+        <v>-3.82</v>
+      </c>
+      <c r="D32" s="3">
+        <v>5.95</v>
+      </c>
+      <c r="G32">
+        <v>0.75</v>
+      </c>
+      <c r="H32">
+        <v>2.5050500000000002</v>
+      </c>
+      <c r="I32">
+        <v>0.13078600000000001</v>
+      </c>
+      <c r="J32">
+        <v>-3.8792399999999998</v>
+      </c>
+      <c r="K32">
+        <v>0.118772</v>
+      </c>
+      <c r="L32">
+        <v>5.8107699999999998</v>
+      </c>
+      <c r="M32">
+        <v>9.8089499999999996E-2</v>
+      </c>
+      <c r="O32" s="1">
+        <f t="shared" si="5"/>
+        <v>-6.0259657060489904E-3</v>
+      </c>
+      <c r="P32" s="1">
+        <f t="shared" si="6"/>
+        <v>-1.5388531855092182E-2</v>
+      </c>
+      <c r="Q32" s="1">
+        <f t="shared" si="7"/>
+        <v>2.367702114742494E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
+      <c r="A33">
+        <v>0.75</v>
+      </c>
+      <c r="B33">
+        <v>3.59</v>
+      </c>
+      <c r="C33" s="3">
+        <v>-3.22</v>
+      </c>
+      <c r="D33" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="G33">
+        <v>0.75</v>
+      </c>
+      <c r="H33">
+        <v>3.6073599999999999</v>
+      </c>
+      <c r="I33">
+        <v>0.184171</v>
+      </c>
+      <c r="J33">
+        <v>-3.2593100000000002</v>
+      </c>
+      <c r="K33">
+        <v>0.17548800000000001</v>
+      </c>
+      <c r="L33">
+        <v>9.0255399999999995</v>
+      </c>
+      <c r="M33">
+        <v>0.138128</v>
+      </c>
+      <c r="O33" s="1">
+        <f t="shared" si="5"/>
+        <v>-4.8239910189291748E-3</v>
+      </c>
+      <c r="P33" s="1">
+        <f t="shared" si="6"/>
+        <v>-1.2134008096541131E-2</v>
+      </c>
+      <c r="Q33" s="1">
+        <f t="shared" si="7"/>
+        <v>1.914456306918751E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="A34">
+        <v>0.65</v>
+      </c>
+      <c r="B34">
+        <v>1.31</v>
+      </c>
+      <c r="C34" s="3">
+        <v>-4.0599999999999996</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0.81</v>
+      </c>
+      <c r="G34">
+        <v>0.65</v>
+      </c>
+      <c r="H34">
+        <v>1.30768</v>
+      </c>
+      <c r="I34">
+        <v>6.8848300000000001E-2</v>
+      </c>
+      <c r="J34">
+        <v>-4.0975999999999999</v>
+      </c>
+      <c r="K34">
+        <v>6.3025399999999995E-2</v>
+      </c>
+      <c r="L34">
+        <v>0.803095</v>
+      </c>
+      <c r="M34">
+        <v>4.4751399999999997E-2</v>
+      </c>
+      <c r="O34" s="1">
+        <f t="shared" si="5"/>
+        <v>1.7725619632652577E-3</v>
+      </c>
+      <c r="P34" s="1">
+        <f t="shared" si="6"/>
+        <v>-9.2183975679122065E-3</v>
+      </c>
+      <c r="Q34" s="1">
+        <f t="shared" si="7"/>
+        <v>8.5611820754512916E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="A35">
+        <v>0.65</v>
+      </c>
+      <c r="B35">
+        <v>2.61</v>
+      </c>
+      <c r="C35" s="3">
+        <v>-3.41</v>
+      </c>
+      <c r="D35" s="3">
+        <v>3.89</v>
+      </c>
+      <c r="G35">
+        <v>0.65</v>
+      </c>
+      <c r="H35">
+        <v>2.6075499999999998</v>
+      </c>
+      <c r="I35">
+        <v>0.124114</v>
+      </c>
+      <c r="J35">
+        <v>-3.4250799999999999</v>
+      </c>
+      <c r="K35">
+        <v>0.109254</v>
+      </c>
+      <c r="L35">
+        <v>3.8471700000000002</v>
+      </c>
+      <c r="M35">
+        <v>8.0674399999999993E-2</v>
+      </c>
+      <c r="O35" s="1">
+        <f t="shared" si="5"/>
+        <v>9.3913810121611237E-4</v>
+      </c>
+      <c r="P35" s="1">
+        <f t="shared" si="6"/>
+        <v>-4.4125306507018973E-3</v>
+      </c>
+      <c r="Q35" s="1">
+        <f t="shared" si="7"/>
+        <v>1.107123147093832E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="A36">
+        <v>0.65</v>
+      </c>
+      <c r="B36">
+        <v>3.79</v>
+      </c>
+      <c r="C36" s="3">
+        <v>-2.94</v>
+      </c>
+      <c r="D36" s="3">
+        <v>6.33</v>
+      </c>
+      <c r="G36">
+        <v>0.65</v>
+      </c>
+      <c r="H36">
+        <v>3.7713399999999999</v>
+      </c>
+      <c r="I36">
+        <v>0.19620399999999999</v>
+      </c>
+      <c r="J36">
+        <v>-2.9329800000000001</v>
+      </c>
+      <c r="K36">
+        <v>0.16444900000000001</v>
+      </c>
+      <c r="L36">
+        <v>6.3543000000000003</v>
+      </c>
+      <c r="M36">
+        <v>0.12753300000000001</v>
+      </c>
+      <c r="O36" s="1">
+        <f t="shared" si="5"/>
+        <v>4.935633102069242E-3</v>
+      </c>
+      <c r="P36" s="1">
+        <f t="shared" si="6"/>
+        <v>2.3906091966939456E-3</v>
+      </c>
+      <c r="Q36" s="1">
+        <f t="shared" si="7"/>
+        <v>-3.8315082424730112E-3</v>
       </c>
     </row>
   </sheetData>
@@ -1052,7 +1727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+    <sheetView topLeftCell="D4" workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added CLI and result logging
</commit_message>
<xml_diff>
--- a/Results/Benchmarking.xlsx
+++ b/Results/Benchmarking.xlsx
@@ -170,17 +170,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="GENERAL" numFmtId="165"/>
-    <numFmt formatCode="0%" numFmtId="166"/>
-    <numFmt formatCode="0.00%" numFmtId="167"/>
-    <numFmt formatCode="0.00" numFmtId="168"/>
-    <numFmt formatCode="0.0%" numFmtId="169"/>
+    <numFmt formatCode="0%" numFmtId="165"/>
+    <numFmt formatCode="0.00%" numFmtId="166"/>
+    <numFmt formatCode="0.00" numFmtId="167"/>
+    <numFmt formatCode="0.0%" numFmtId="168"/>
   </numFmts>
   <fonts count="5">
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
       <color rgb="00000000"/>
       <sz val="11"/>
@@ -201,9 +201,8 @@
       <sz val="10"/>
     </font>
     <font>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <color rgb="00000000"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -247,21 +246,21 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="166">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="165">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="19">
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="19">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="168" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="169" xfId="19">
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="168" xfId="19">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -431,11 +430,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="56132166"/>
-        <c:axId val="92175182"/>
+        <c:axId val="44587649"/>
+        <c:axId val="93868372"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56132166"/>
+        <c:axId val="44587649"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -443,7 +442,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92175182"/>
+        <c:crossAx val="93868372"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln w="9360">
@@ -455,7 +454,7 @@
         </c:spPr>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92175182"/>
+        <c:axId val="93868372"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -473,7 +472,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56132166"/>
+        <c:crossAx val="44587649"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln w="9360">
@@ -505,15 +504,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>560520</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>111960</xdr:rowOff>
+      <xdr:colOff>587520</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>67680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>126000</xdr:rowOff>
+      <xdr:colOff>272520</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>116640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -521,8 +520,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6940440" y="2591640"/>
-        <a:ext cx="8757360" cy="3733920"/>
+        <a:off x="6994080" y="2370240"/>
+        <a:ext cx="8794800" cy="3414600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -542,14 +541,14 @@
   </sheetPr>
   <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="F12" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="I36" activeCellId="0" pane="topLeft" sqref="I36"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="M12" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
+      <selection activeCell="R36" activeCellId="0" pane="topLeft" sqref="R36"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="17" min="1" style="0" width="8.56862745098039"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.89411764705882"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="17" min="1" style="0" width="8.60392156862745"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.93725490196078"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -1847,9 +1846,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.56862745098039"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.3333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.60392156862745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.3843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -2622,7 +2621,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>